<commit_message>
updated spring start indices
start indices for spring trials
</commit_message>
<xml_diff>
--- a/Code/Matlab/Analysis/DampedLeg_Krnacik/Haonan/3DPrinted_Torsion_Spring/torqueTest/data/SpringStartIndex.xlsx
+++ b/Code/Matlab/Analysis/DampedLeg_Krnacik/Haonan/3DPrinted_Torsion_Spring/torqueTest/data/SpringStartIndex.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Quadruped_Robot\Code\Matlab\Analysis\DampedLeg_Krnacik\Haonan\3DPrinted_Torsion_Spring\torqueTest\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Quadruped_Robot\Code\Matlab\Analysis\DampedLeg_Krnacik\Haonan\3DPrinted_Torsion_Spring\torqueTest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCBB7C5-5B94-4B63-82AE-7717F9DDB67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3739EF4-C25D-46D5-8836-70916CB74879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28905" yWindow="-15" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2L2LT4ST_37T" sheetId="1" r:id="rId1"/>
@@ -410,13 +410,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -446,8 +446,11 @@
       <c r="E2">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F2">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>6</v>
@@ -461,8 +464,11 @@
       <c r="E3">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F3">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>7</v>
@@ -476,8 +482,11 @@
       <c r="E4">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>8</v>
@@ -491,8 +500,11 @@
       <c r="E5">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>9</v>
@@ -506,8 +518,11 @@
       <c r="E6">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F6">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>10</v>
@@ -521,8 +536,11 @@
       <c r="E7">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>11</v>
@@ -536,8 +554,11 @@
       <c r="E8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>12</v>
@@ -551,8 +572,11 @@
       <c r="E9">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F9">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -568,8 +592,11 @@
       <c r="E10">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F10">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>6</v>
@@ -583,8 +610,11 @@
       <c r="E11">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F11">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>7</v>
@@ -598,8 +628,11 @@
       <c r="E12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F12">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
         <v>8</v>
@@ -613,8 +646,11 @@
       <c r="E13">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F13">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
         <v>9</v>
@@ -628,8 +664,11 @@
       <c r="E14">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F14">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
         <v>10</v>
@@ -643,8 +682,11 @@
       <c r="E15">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F15">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
         <v>11</v>
@@ -658,8 +700,11 @@
       <c r="E16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>12</v>
@@ -672,6 +717,9 @@
       </c>
       <c r="E17">
         <v>0.18</v>
+      </c>
+      <c r="F17">
+        <v>0.17</v>
       </c>
     </row>
   </sheetData>
@@ -689,12 +737,12 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>1</v>
       </c>
@@ -708,104 +756,296 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <v>0.16</v>
+      </c>
+      <c r="D2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E2">
+        <v>0.37</v>
+      </c>
+      <c r="F2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0.36</v>
+      </c>
+      <c r="F3">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>0.21</v>
+      </c>
+      <c r="D4">
+        <v>0.22</v>
+      </c>
+      <c r="E4">
+        <v>0.26</v>
+      </c>
+      <c r="F4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>0.12</v>
+      </c>
+      <c r="D5">
+        <v>0.32</v>
+      </c>
+      <c r="E5">
+        <v>0.02</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>0.12</v>
+      </c>
+      <c r="D6">
+        <v>0.08</v>
+      </c>
+      <c r="E6">
+        <v>0.2</v>
+      </c>
+      <c r="F6">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.09</v>
+      </c>
+      <c r="E7">
+        <v>0.18</v>
+      </c>
+      <c r="F7">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>0.09</v>
+      </c>
+      <c r="D8">
+        <v>0.25</v>
+      </c>
+      <c r="E8">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F8">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <v>0.12</v>
+      </c>
+      <c r="D9">
+        <v>0.17</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <v>0.11</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0.05</v>
+      </c>
+      <c r="F10">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C11">
+        <v>0.17</v>
+      </c>
+      <c r="D11">
+        <v>0.25</v>
+      </c>
+      <c r="E11">
+        <v>0.15</v>
+      </c>
+      <c r="F11">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <v>0.03</v>
+      </c>
+      <c r="D12">
+        <v>0.17</v>
+      </c>
+      <c r="E12">
+        <v>0.22</v>
+      </c>
+      <c r="F12">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C13">
+        <v>0.17</v>
+      </c>
+      <c r="D13">
+        <v>0.05</v>
+      </c>
+      <c r="E13">
+        <v>0.2</v>
+      </c>
+      <c r="F13">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <v>0.11</v>
+      </c>
+      <c r="D14">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F14">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C15">
+        <v>0.25</v>
+      </c>
+      <c r="D15">
+        <v>0.26</v>
+      </c>
+      <c r="E15">
+        <v>0.18</v>
+      </c>
+      <c r="F15">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <v>0.27</v>
+      </c>
+      <c r="D16">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E16">
+        <v>0.2</v>
+      </c>
+      <c r="F16">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>12</v>
+      </c>
+      <c r="C17">
+        <v>0.06</v>
+      </c>
+      <c r="D17">
+        <v>0.54</v>
+      </c>
+      <c r="E17">
+        <v>0.05</v>
+      </c>
+      <c r="F17">
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>
@@ -821,13 +1061,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B95A850-7988-4D99-B418-55343BCF56E6}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>2</v>
       </c>
@@ -841,7 +1081,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -849,49 +1089,49 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -899,43 +1139,43 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>12</v>
@@ -958,9 +1198,9 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>17</v>
       </c>
@@ -974,7 +1214,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -982,49 +1222,49 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1032,43 +1272,43 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
update spring start indices
update data file
</commit_message>
<xml_diff>
--- a/Code/Matlab/Analysis/DampedLeg_Krnacik/Haonan/3DPrinted_Torsion_Spring/torqueTest/data/SpringStartIndex.xlsx
+++ b/Code/Matlab/Analysis/DampedLeg_Krnacik/Haonan/3DPrinted_Torsion_Spring/torqueTest/data/SpringStartIndex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Quadruped_Robot\Code\Matlab\Analysis\DampedLeg_Krnacik\Haonan\3DPrinted_Torsion_Spring\torqueTest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3739EF4-C25D-46D5-8836-70916CB74879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25C896E-5B5E-4B9E-8280-17ACD5E58000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="-15" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2L2LT4ST_37T" sheetId="1" r:id="rId1"/>
@@ -1062,7 +1062,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,48 +1088,144 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
+      <c r="C2">
+        <v>0.09</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0.17</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>6</v>
       </c>
+      <c r="C3">
+        <v>0.19</v>
+      </c>
+      <c r="D3">
+        <v>0.36</v>
+      </c>
+      <c r="E3">
+        <v>0.17</v>
+      </c>
+      <c r="F3">
+        <v>0.33500000000000002</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="C4">
+        <v>0.19</v>
+      </c>
+      <c r="D4">
+        <v>0.17</v>
+      </c>
+      <c r="E4">
+        <v>0.21</v>
+      </c>
+      <c r="F4">
+        <v>0.04</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>8</v>
       </c>
+      <c r="C5">
+        <v>0.09</v>
+      </c>
+      <c r="D5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E5">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.41</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>9</v>
       </c>
+      <c r="C6">
+        <v>0.15</v>
+      </c>
+      <c r="D6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0.16</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>10</v>
       </c>
+      <c r="C7">
+        <v>0.11</v>
+      </c>
+      <c r="D7">
+        <v>0.17</v>
+      </c>
+      <c r="E7">
+        <v>0.12</v>
+      </c>
+      <c r="F7">
+        <v>0.24</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>11</v>
       </c>
+      <c r="C8">
+        <v>0.18</v>
+      </c>
+      <c r="D8">
+        <v>0.16</v>
+      </c>
+      <c r="E8">
+        <v>0.12</v>
+      </c>
+      <c r="F8">
+        <v>0.13</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>12</v>
       </c>
+      <c r="C9">
+        <v>0.17</v>
+      </c>
+      <c r="D9">
+        <v>0.18</v>
+      </c>
+      <c r="E9">
+        <v>0.21</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1137,6 +1233,18 @@
       </c>
       <c r="B10" t="s">
         <v>5</v>
+      </c>
+      <c r="C10">
+        <v>0.12</v>
+      </c>
+      <c r="D10">
+        <v>0.02</v>
+      </c>
+      <c r="E10">
+        <v>0.19</v>
+      </c>
+      <c r="F10">
+        <v>0.16</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1144,41 +1252,125 @@
       <c r="B11" t="s">
         <v>6</v>
       </c>
+      <c r="C11">
+        <v>0.1</v>
+      </c>
+      <c r="D11">
+        <v>0.17</v>
+      </c>
+      <c r="E11">
+        <v>0.11</v>
+      </c>
+      <c r="F11">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>7</v>
       </c>
+      <c r="C12">
+        <v>0.27</v>
+      </c>
+      <c r="D12">
+        <v>0.15</v>
+      </c>
+      <c r="E12">
+        <v>0.1</v>
+      </c>
+      <c r="F12">
+        <v>0.11</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
         <v>8</v>
       </c>
+      <c r="C13">
+        <v>0.18</v>
+      </c>
+      <c r="D13">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E13">
+        <v>0.21</v>
+      </c>
+      <c r="F13">
+        <v>0.27</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
         <v>9</v>
       </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0.18</v>
+      </c>
+      <c r="E14">
+        <v>0.23</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
         <v>10</v>
       </c>
+      <c r="C15">
+        <v>0.13</v>
+      </c>
+      <c r="D15">
+        <v>0.12</v>
+      </c>
+      <c r="E15">
+        <v>0.13</v>
+      </c>
+      <c r="F15">
+        <v>0.27</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>0.23</v>
+      </c>
+      <c r="D16">
+        <v>0.11</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>12</v>
+      </c>
+      <c r="C17">
+        <v>0.23</v>
+      </c>
+      <c r="D17">
+        <v>0.15</v>
+      </c>
+      <c r="E17">
+        <v>0.16</v>
+      </c>
+      <c r="F17">
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>